<commit_message>
Adding data observability code
</commit_message>
<xml_diff>
--- a/Accelerator/Data Observability/Output/client_dim.xlsx
+++ b/Accelerator/Data Observability/Output/client_dim.xlsx
@@ -9,6 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Drift" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Numerical" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Categorical" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Usage" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -485,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +550,11 @@
           <t>Median</t>
         </is>
       </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>skewness</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -557,7 +563,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -572,19 +578,22 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>15678</v>
+        <v>15755</v>
       </c>
       <c r="J2" t="n">
-        <v>7802.38</v>
+        <v>7841.89</v>
       </c>
       <c r="K2" t="n">
-        <v>7537.5</v>
+        <v>7573.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.06</v>
       </c>
     </row>
     <row r="3">
@@ -594,7 +603,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5302</v>
+        <v>5321</v>
       </c>
       <c r="C3" t="n">
         <v>10</v>
@@ -603,13 +612,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>8242</v>
+        <v>8291</v>
       </c>
       <c r="F3" t="n">
-        <v>60.85</v>
+        <v>60.91</v>
       </c>
       <c r="G3" t="n">
-        <v>2080</v>
+        <v>2087</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -618,10 +627,13 @@
         <v>584625</v>
       </c>
       <c r="J3" t="n">
-        <v>20716.02</v>
+        <v>20701.87</v>
       </c>
       <c r="K3" t="n">
-        <v>8489</v>
+        <v>8500</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5.71</v>
       </c>
     </row>
     <row r="4">
@@ -631,7 +643,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5304</v>
+        <v>5323</v>
       </c>
       <c r="C4" t="n">
         <v>5</v>
@@ -640,26 +652,29 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>8240</v>
+        <v>8289</v>
       </c>
       <c r="F4" t="n">
-        <v>60.84</v>
+        <v>60.89</v>
       </c>
       <c r="G4" t="n">
-        <v>2722</v>
+        <v>2731</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>2658290.5</v>
+        <v>2670982.5</v>
       </c>
       <c r="J4" t="n">
-        <v>34163.02</v>
+        <v>34200.25</v>
       </c>
       <c r="K4" t="n">
         <v>12000</v>
       </c>
+      <c r="L4" t="n">
+        <v>12.29</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -668,7 +683,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4923</v>
+        <v>4938</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -677,13 +692,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>8621</v>
+        <v>8674</v>
       </c>
       <c r="F5" t="n">
-        <v>63.65</v>
+        <v>63.72</v>
       </c>
       <c r="G5" t="n">
-        <v>3481</v>
+        <v>3491</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -692,10 +707,13 @@
         <v>984026.05</v>
       </c>
       <c r="J5" t="n">
-        <v>16782.16</v>
+        <v>16807.41</v>
       </c>
       <c r="K5" t="n">
-        <v>5869.2</v>
+        <v>5877.5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>9.15</v>
       </c>
     </row>
     <row r="6">
@@ -705,7 +723,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4937</v>
+        <v>4952</v>
       </c>
       <c r="C6" t="n">
         <v>104</v>
@@ -714,26 +732,29 @@
         <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>8607</v>
+        <v>8660</v>
       </c>
       <c r="F6" t="n">
-        <v>63.55</v>
+        <v>63.62</v>
       </c>
       <c r="G6" t="n">
-        <v>1643</v>
+        <v>1670</v>
       </c>
       <c r="H6" t="n">
         <v>-5700</v>
       </c>
       <c r="I6" t="n">
-        <v>153620</v>
+        <v>211833</v>
       </c>
       <c r="J6" t="n">
-        <v>1989.98</v>
+        <v>2050.41</v>
       </c>
       <c r="K6" t="n">
         <v>700</v>
       </c>
+      <c r="L6" t="n">
+        <v>15.51</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -742,7 +763,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7085</v>
+        <v>7104</v>
       </c>
       <c r="C7" t="n">
         <v>1781</v>
@@ -751,10 +772,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>6459</v>
+        <v>6508</v>
       </c>
       <c r="F7" t="n">
-        <v>47.69</v>
+        <v>47.81</v>
       </c>
       <c r="G7" t="n">
         <v>31</v>
@@ -763,14 +784,17 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>384</v>
+        <v>427</v>
       </c>
       <c r="J7" t="n">
-        <v>2.17</v>
+        <v>2.18</v>
       </c>
       <c r="K7" t="n">
         <v>2</v>
       </c>
+      <c r="L7" t="n">
+        <v>59.68</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -779,19 +803,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7085</v>
+        <v>7104</v>
       </c>
       <c r="C8" t="n">
-        <v>4130</v>
+        <v>4148</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>6459</v>
+        <v>6508</v>
       </c>
       <c r="F8" t="n">
-        <v>47.69</v>
+        <v>47.81</v>
       </c>
       <c r="G8" t="n">
         <v>10</v>
@@ -808,6 +832,9 @@
       <c r="K8" t="n">
         <v>0</v>
       </c>
+      <c r="L8" t="n">
+        <v>2.43</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -816,7 +843,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>7085</v>
+        <v>7104</v>
       </c>
       <c r="C9" t="n">
         <v>1781</v>
@@ -825,10 +852,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>6459</v>
+        <v>6508</v>
       </c>
       <c r="F9" t="n">
-        <v>47.69</v>
+        <v>47.81</v>
       </c>
       <c r="G9" t="n">
         <v>17</v>
@@ -837,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="J9" t="n">
         <v>1.1</v>
@@ -845,6 +872,9 @@
       <c r="K9" t="n">
         <v>1</v>
       </c>
+      <c r="L9" t="n">
+        <v>21.53</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -853,19 +883,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7085</v>
+        <v>7104</v>
       </c>
       <c r="C10" t="n">
-        <v>5757</v>
+        <v>5762</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>6459</v>
+        <v>6508</v>
       </c>
       <c r="F10" t="n">
-        <v>47.69</v>
+        <v>47.81</v>
       </c>
       <c r="G10" t="n">
         <v>10</v>
@@ -874,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="J10" t="n">
         <v>0.22</v>
@@ -882,6 +912,9 @@
       <c r="K10" t="n">
         <v>0</v>
       </c>
+      <c r="L10" t="n">
+        <v>31.51</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -899,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="F11" t="n">
         <v>100</v>
@@ -924,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="F12" t="n">
         <v>100</v>
@@ -949,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="F13" t="n">
         <v>100</v>
@@ -974,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="F14" t="n">
         <v>100</v>
@@ -999,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="F15" t="n">
         <v>100</v>
@@ -1024,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="F16" t="n">
         <v>100</v>
@@ -1049,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="F17" t="n">
         <v>100</v>
@@ -1065,7 +1098,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -1074,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>13153</v>
+        <v>13216</v>
       </c>
       <c r="F18" t="n">
-        <v>97.11</v>
+        <v>97.09</v>
       </c>
       <c r="G18" t="n">
         <v>4</v>
@@ -1094,6 +1127,9 @@
       <c r="K18" t="n">
         <v>1</v>
       </c>
+      <c r="L18" t="n">
+        <v>6.04</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1102,22 +1138,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="C19" t="n">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>13153</v>
+        <v>13216</v>
       </c>
       <c r="F19" t="n">
-        <v>97.11</v>
+        <v>97.09</v>
       </c>
       <c r="G19" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1126,10 +1162,13 @@
         <v>480000</v>
       </c>
       <c r="J19" t="n">
-        <v>13255.26</v>
+        <v>11727.75</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>7.39</v>
       </c>
     </row>
     <row r="20">
@@ -1139,7 +1178,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1328</v>
+        <v>1342</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -1148,10 +1187,10 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>12216</v>
+        <v>12270</v>
       </c>
       <c r="F20" t="n">
-        <v>90.19</v>
+        <v>90.14</v>
       </c>
       <c r="G20" t="n">
         <v>13</v>
@@ -1160,13 +1199,16 @@
         <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>192</v>
+        <v>235</v>
       </c>
       <c r="J20" t="n">
-        <v>1.64</v>
+        <v>1.68</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
+      </c>
+      <c r="L20" t="n">
+        <v>35.23</v>
       </c>
     </row>
   </sheetData>
@@ -1232,16 +1274,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5303</v>
+        <v>5322</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>8241</v>
+        <v>8290</v>
       </c>
       <c r="E2" t="n">
-        <v>60.85</v>
+        <v>60.9</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
@@ -1259,7 +1301,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13530</v>
+        <v>13598</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -1286,7 +1328,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13530</v>
+        <v>13598</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -1313,16 +1355,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13530</v>
+        <v>13576</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
@@ -1340,7 +1382,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13264</v>
+        <v>13332</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1349,7 +1391,7 @@
         <v>280</v>
       </c>
       <c r="E6" t="n">
-        <v>2.07</v>
+        <v>2.06</v>
       </c>
       <c r="F6" t="n">
         <v>4</v>
@@ -1367,16 +1409,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7085</v>
+        <v>7104</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6459</v>
+        <v>6508</v>
       </c>
       <c r="E7" t="n">
-        <v>47.69</v>
+        <v>47.81</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
@@ -1394,7 +1436,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -1421,7 +1463,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -1448,7 +1490,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>13544</v>
+        <v>13612</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -1465,6 +1507,83 @@
       <c r="G10" t="inlineStr">
         <is>
           <t>1-10</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>schemaname</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>no_of_times_accessed</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>table_name</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>indexrelname</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>tables_usability</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>index_usability</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>adaptiveai</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>45</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>client_dim</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Used</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Index not used</t>
         </is>
       </c>
     </row>

</xml_diff>